<commit_message>
Connection Service diagram update
</commit_message>
<xml_diff>
--- a/Modeli pretnji/ConnectionService.xlsx
+++ b/Modeli pretnji/ConnectionService.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A2A419-55B5-4519-ABF4-6919321F1D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5E5C41-7C95-49BD-B0BE-E92F05F631A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -1057,15 +1057,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1111,20 +1126,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1132,58 +1162,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1193,15 +1202,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1223,45 +1223,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>426721</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>45721</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="4663984" cy="4090634"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{209382B8-037F-4E28-9DD8-F8379C28E9EB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1889761" y="3886201"/>
-          <a:ext cx="4663984" cy="4090634"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -1289,7 +1250,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1333,7 +1294,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1342,6 +1303,50 @@
         <a:xfrm>
           <a:off x="929640" y="3901440"/>
           <a:ext cx="6421113" cy="4069080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>279885</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>157915</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD377B8C-207E-86C2-F118-69436F004F88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1912620" y="8267701"/>
+          <a:ext cx="4707105" cy="4143174"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1780,19 +1785,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="E1" s="55" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="E1" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -1804,27 +1809,27 @@
       <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="56"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="58"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="63"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20">
         <v>1</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="61"/>
+      <c r="C3" s="59"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="66"/>
     </row>
     <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
@@ -1836,12 +1841,12 @@
       <c r="C4" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="59"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="61"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="66"/>
     </row>
     <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -1853,12 +1858,12 @@
       <c r="C5" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="61"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="66"/>
     </row>
     <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
@@ -1870,27 +1875,27 @@
       <c r="C6" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="61"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="66"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>2</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="61"/>
+      <c r="C7" s="57"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="66"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -1902,12 +1907,12 @@
       <c r="C8" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="61"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="66"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
@@ -1919,27 +1924,27 @@
       <c r="C9" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E9" s="59"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="61"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="66"/>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>3</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="61"/>
+      <c r="C10" s="57"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="66"/>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
@@ -1951,12 +1956,12 @@
       <c r="C11" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="E11" s="59"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="61"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="66"/>
     </row>
     <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
@@ -1968,12 +1973,12 @@
       <c r="C12" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="59"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="61"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="66"/>
     </row>
     <row r="13" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
@@ -1985,25 +1990,25 @@
       <c r="C13" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E13" s="62"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="64"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="69"/>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="55"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
@@ -2015,7 +2020,7 @@
       <c r="C15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="48" t="s">
+      <c r="E15" s="54" t="s">
         <v>58</v>
       </c>
       <c r="F15" s="49"/>
@@ -2076,26 +2081,26 @@
       <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="67" t="s">
+      <c r="B20" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="68"/>
+      <c r="C20" s="51"/>
       <c r="E20" s="49"/>
       <c r="F20" s="49"/>
       <c r="G20" s="49"/>
@@ -2107,10 +2112,10 @@
       <c r="A21" s="14">
         <v>1</v>
       </c>
-      <c r="B21" s="65" t="s">
+      <c r="B21" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="65"/>
+      <c r="C21" s="47"/>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
       <c r="G21" s="49"/>
@@ -2122,10 +2127,10 @@
       <c r="A22" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="66" t="s">
+      <c r="B22" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="66"/>
+      <c r="C22" s="48"/>
       <c r="E22" s="49"/>
       <c r="F22" s="49"/>
       <c r="G22" s="49"/>
@@ -2137,10 +2142,10 @@
       <c r="A23" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="66"/>
+      <c r="C23" s="48"/>
       <c r="E23" s="49"/>
       <c r="F23" s="49"/>
       <c r="G23" s="49"/>
@@ -2152,10 +2157,10 @@
       <c r="A24" s="14">
         <v>2</v>
       </c>
-      <c r="B24" s="65" t="s">
+      <c r="B24" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="65"/>
+      <c r="C24" s="47"/>
       <c r="E24" s="49"/>
       <c r="F24" s="49"/>
       <c r="G24" s="49"/>
@@ -2167,10 +2172,10 @@
       <c r="A25" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="69" t="s">
+      <c r="B25" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="69"/>
+      <c r="C25" s="52"/>
       <c r="E25" s="49"/>
       <c r="F25" s="49"/>
       <c r="G25" s="49"/>
@@ -2182,10 +2187,10 @@
       <c r="A26" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="69" t="s">
+      <c r="B26" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="C26" s="69"/>
+      <c r="C26" s="52"/>
       <c r="E26" s="49"/>
       <c r="F26" s="49"/>
       <c r="G26" s="49"/>
@@ -2195,14 +2200,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E20:J26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
     <mergeCell ref="E14:J14"/>
     <mergeCell ref="E15:J18"/>
     <mergeCell ref="E19:J19"/>
@@ -2214,6 +2211,14 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E1:J1"/>
     <mergeCell ref="E2:J13"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E20:J26"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2224,7 +2229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:T68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P56" sqref="P56"/>
     </sheetView>
   </sheetViews>
@@ -2234,1255 +2239,1255 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
       <c r="O1" s="1"/>
-      <c r="P1" s="55" t="s">
+      <c r="P1" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
     </row>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="P2" s="48" t="s">
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="P2" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="80"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="70"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="P3" s="80"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="80"/>
+      <c r="S3" s="80"/>
+      <c r="T3" s="80"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="P4" s="70"/>
-      <c r="Q4" s="70"/>
-      <c r="R4" s="70"/>
-      <c r="S4" s="70"/>
-      <c r="T4" s="70"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="P4" s="80"/>
+      <c r="Q4" s="80"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="80"/>
+      <c r="T4" s="80"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="P5" s="70"/>
-      <c r="Q5" s="70"/>
-      <c r="R5" s="70"/>
-      <c r="S5" s="70"/>
-      <c r="T5" s="70"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="P5" s="80"/>
+      <c r="Q5" s="80"/>
+      <c r="R5" s="80"/>
+      <c r="S5" s="80"/>
+      <c r="T5" s="80"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
-      <c r="N6" s="73"/>
-      <c r="P6" s="70"/>
-      <c r="Q6" s="70"/>
-      <c r="R6" s="70"/>
-      <c r="S6" s="70"/>
-      <c r="T6" s="70"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="82"/>
+      <c r="P6" s="80"/>
+      <c r="Q6" s="80"/>
+      <c r="R6" s="80"/>
+      <c r="S6" s="80"/>
+      <c r="T6" s="80"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="73"/>
-      <c r="P7" s="70"/>
-      <c r="Q7" s="70"/>
-      <c r="R7" s="70"/>
-      <c r="S7" s="70"/>
-      <c r="T7" s="70"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
+      <c r="P7" s="80"/>
+      <c r="Q7" s="80"/>
+      <c r="R7" s="80"/>
+      <c r="S7" s="80"/>
+      <c r="T7" s="80"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="73"/>
-      <c r="P8" s="70"/>
-      <c r="Q8" s="70"/>
-      <c r="R8" s="70"/>
-      <c r="S8" s="70"/>
-      <c r="T8" s="70"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="82"/>
+      <c r="L8" s="82"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="82"/>
+      <c r="P8" s="80"/>
+      <c r="Q8" s="80"/>
+      <c r="R8" s="80"/>
+      <c r="S8" s="80"/>
+      <c r="T8" s="80"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73"/>
-      <c r="N9" s="73"/>
-      <c r="P9" s="70"/>
-      <c r="Q9" s="70"/>
-      <c r="R9" s="70"/>
-      <c r="S9" s="70"/>
-      <c r="T9" s="70"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="82"/>
+      <c r="K9" s="82"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="82"/>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="80"/>
+      <c r="R9" s="80"/>
+      <c r="S9" s="80"/>
+      <c r="T9" s="80"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
-      <c r="P10" s="70"/>
-      <c r="Q10" s="70"/>
-      <c r="R10" s="70"/>
-      <c r="S10" s="70"/>
-      <c r="T10" s="70"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="82"/>
+      <c r="P10" s="80"/>
+      <c r="Q10" s="80"/>
+      <c r="R10" s="80"/>
+      <c r="S10" s="80"/>
+      <c r="T10" s="80"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B11" s="73"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
-      <c r="P11" s="70"/>
-      <c r="Q11" s="70"/>
-      <c r="R11" s="70"/>
-      <c r="S11" s="70"/>
-      <c r="T11" s="70"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="82"/>
+      <c r="P11" s="80"/>
+      <c r="Q11" s="80"/>
+      <c r="R11" s="80"/>
+      <c r="S11" s="80"/>
+      <c r="T11" s="80"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
-      <c r="J12" s="73"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="73"/>
-      <c r="M12" s="73"/>
-      <c r="N12" s="73"/>
-      <c r="P12" s="70"/>
-      <c r="Q12" s="70"/>
-      <c r="R12" s="70"/>
-      <c r="S12" s="70"/>
-      <c r="T12" s="70"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
+      <c r="P12" s="80"/>
+      <c r="Q12" s="80"/>
+      <c r="R12" s="80"/>
+      <c r="S12" s="80"/>
+      <c r="T12" s="80"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="73"/>
-      <c r="L13" s="73"/>
-      <c r="M13" s="73"/>
-      <c r="N13" s="73"/>
-      <c r="P13" s="70"/>
-      <c r="Q13" s="70"/>
-      <c r="R13" s="70"/>
-      <c r="S13" s="70"/>
-      <c r="T13" s="70"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="82"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
+      <c r="P13" s="80"/>
+      <c r="Q13" s="80"/>
+      <c r="R13" s="80"/>
+      <c r="S13" s="80"/>
+      <c r="T13" s="80"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="73"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="73"/>
-      <c r="L14" s="73"/>
-      <c r="M14" s="73"/>
-      <c r="N14" s="73"/>
-      <c r="P14" s="70"/>
-      <c r="Q14" s="70"/>
-      <c r="R14" s="70"/>
-      <c r="S14" s="70"/>
-      <c r="T14" s="70"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="82"/>
+      <c r="P14" s="80"/>
+      <c r="Q14" s="80"/>
+      <c r="R14" s="80"/>
+      <c r="S14" s="80"/>
+      <c r="T14" s="80"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B15" s="73"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="73"/>
-      <c r="N15" s="73"/>
-      <c r="P15" s="70"/>
-      <c r="Q15" s="70"/>
-      <c r="R15" s="70"/>
-      <c r="S15" s="70"/>
-      <c r="T15" s="70"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="82"/>
+      <c r="K15" s="82"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="82"/>
+      <c r="N15" s="82"/>
+      <c r="P15" s="80"/>
+      <c r="Q15" s="80"/>
+      <c r="R15" s="80"/>
+      <c r="S15" s="80"/>
+      <c r="T15" s="80"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="73"/>
-      <c r="N16" s="73"/>
-      <c r="P16" s="70"/>
-      <c r="Q16" s="70"/>
-      <c r="R16" s="70"/>
-      <c r="S16" s="70"/>
-      <c r="T16" s="70"/>
+      <c r="B16" s="82"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="82"/>
+      <c r="F16" s="82"/>
+      <c r="G16" s="82"/>
+      <c r="H16" s="82"/>
+      <c r="I16" s="82"/>
+      <c r="J16" s="82"/>
+      <c r="K16" s="82"/>
+      <c r="L16" s="82"/>
+      <c r="M16" s="82"/>
+      <c r="N16" s="82"/>
+      <c r="P16" s="80"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="80"/>
+      <c r="S16" s="80"/>
+      <c r="T16" s="80"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B17" s="73"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="73"/>
-      <c r="J17" s="73"/>
-      <c r="K17" s="73"/>
-      <c r="L17" s="73"/>
-      <c r="M17" s="73"/>
-      <c r="N17" s="73"/>
-      <c r="P17" s="70"/>
-      <c r="Q17" s="70"/>
-      <c r="R17" s="70"/>
-      <c r="S17" s="70"/>
-      <c r="T17" s="70"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="82"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="82"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="82"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="82"/>
+      <c r="N17" s="82"/>
+      <c r="P17" s="80"/>
+      <c r="Q17" s="80"/>
+      <c r="R17" s="80"/>
+      <c r="S17" s="80"/>
+      <c r="T17" s="80"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="73"/>
-      <c r="K18" s="73"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="73"/>
-      <c r="N18" s="73"/>
-      <c r="P18" s="70"/>
-      <c r="Q18" s="70"/>
-      <c r="R18" s="70"/>
-      <c r="S18" s="70"/>
-      <c r="T18" s="70"/>
+      <c r="B18" s="82"/>
+      <c r="C18" s="82"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="82"/>
+      <c r="G18" s="82"/>
+      <c r="H18" s="82"/>
+      <c r="I18" s="82"/>
+      <c r="J18" s="82"/>
+      <c r="K18" s="82"/>
+      <c r="L18" s="82"/>
+      <c r="M18" s="82"/>
+      <c r="N18" s="82"/>
+      <c r="P18" s="80"/>
+      <c r="Q18" s="80"/>
+      <c r="R18" s="80"/>
+      <c r="S18" s="80"/>
+      <c r="T18" s="80"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="73"/>
-      <c r="K19" s="73"/>
-      <c r="L19" s="73"/>
-      <c r="M19" s="73"/>
-      <c r="N19" s="73"/>
-      <c r="P19" s="70"/>
-      <c r="Q19" s="70"/>
-      <c r="R19" s="70"/>
-      <c r="S19" s="70"/>
-      <c r="T19" s="70"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="82"/>
+      <c r="H19" s="82"/>
+      <c r="I19" s="82"/>
+      <c r="J19" s="82"/>
+      <c r="K19" s="82"/>
+      <c r="L19" s="82"/>
+      <c r="M19" s="82"/>
+      <c r="N19" s="82"/>
+      <c r="P19" s="80"/>
+      <c r="Q19" s="80"/>
+      <c r="R19" s="80"/>
+      <c r="S19" s="80"/>
+      <c r="T19" s="80"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B20" s="73"/>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="73"/>
-      <c r="I20" s="73"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="73"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="73"/>
-      <c r="N20" s="73"/>
-      <c r="P20" s="70"/>
-      <c r="Q20" s="70"/>
-      <c r="R20" s="70"/>
-      <c r="S20" s="70"/>
-      <c r="T20" s="70"/>
+      <c r="B20" s="82"/>
+      <c r="C20" s="82"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="82"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="82"/>
+      <c r="K20" s="82"/>
+      <c r="L20" s="82"/>
+      <c r="M20" s="82"/>
+      <c r="N20" s="82"/>
+      <c r="P20" s="80"/>
+      <c r="Q20" s="80"/>
+      <c r="R20" s="80"/>
+      <c r="S20" s="80"/>
+      <c r="T20" s="80"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B21" s="72" t="s">
+      <c r="B21" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="72"/>
-      <c r="L21" s="72"/>
-      <c r="M21" s="72"/>
-      <c r="N21" s="72"/>
-      <c r="P21" s="47"/>
-      <c r="Q21" s="47"/>
-      <c r="R21" s="47"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="47"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="70"/>
+      <c r="L21" s="70"/>
+      <c r="M21" s="70"/>
+      <c r="N21" s="70"/>
+      <c r="P21" s="53"/>
+      <c r="Q21" s="53"/>
+      <c r="R21" s="53"/>
+      <c r="S21" s="53"/>
+      <c r="T21" s="53"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B22" s="74"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="75"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="75"/>
-      <c r="K22" s="75"/>
-      <c r="L22" s="75"/>
-      <c r="M22" s="75"/>
-      <c r="N22" s="76"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="72"/>
+      <c r="K22" s="72"/>
+      <c r="L22" s="72"/>
+      <c r="M22" s="72"/>
+      <c r="N22" s="73"/>
       <c r="P22" s="49"/>
-      <c r="Q22" s="71"/>
-      <c r="R22" s="71"/>
-      <c r="S22" s="71"/>
-      <c r="T22" s="71"/>
+      <c r="Q22" s="81"/>
+      <c r="R22" s="81"/>
+      <c r="S22" s="81"/>
+      <c r="T22" s="81"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B23" s="77"/>
-      <c r="C23" s="78"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="78"/>
-      <c r="L23" s="78"/>
-      <c r="M23" s="78"/>
-      <c r="N23" s="79"/>
-      <c r="P23" s="71"/>
-      <c r="Q23" s="71"/>
-      <c r="R23" s="71"/>
-      <c r="S23" s="71"/>
-      <c r="T23" s="71"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="75"/>
+      <c r="L23" s="75"/>
+      <c r="M23" s="75"/>
+      <c r="N23" s="76"/>
+      <c r="P23" s="81"/>
+      <c r="Q23" s="81"/>
+      <c r="R23" s="81"/>
+      <c r="S23" s="81"/>
+      <c r="T23" s="81"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B24" s="77"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="78"/>
-      <c r="K24" s="78"/>
-      <c r="L24" s="78"/>
-      <c r="M24" s="78"/>
-      <c r="N24" s="79"/>
-      <c r="P24" s="71"/>
-      <c r="Q24" s="71"/>
-      <c r="R24" s="71"/>
-      <c r="S24" s="71"/>
-      <c r="T24" s="71"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="75"/>
+      <c r="J24" s="75"/>
+      <c r="K24" s="75"/>
+      <c r="L24" s="75"/>
+      <c r="M24" s="75"/>
+      <c r="N24" s="76"/>
+      <c r="P24" s="81"/>
+      <c r="Q24" s="81"/>
+      <c r="R24" s="81"/>
+      <c r="S24" s="81"/>
+      <c r="T24" s="81"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B25" s="77"/>
-      <c r="C25" s="78"/>
-      <c r="D25" s="78"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="78"/>
-      <c r="H25" s="78"/>
-      <c r="I25" s="78"/>
-      <c r="J25" s="78"/>
-      <c r="K25" s="78"/>
-      <c r="L25" s="78"/>
-      <c r="M25" s="78"/>
-      <c r="N25" s="79"/>
-      <c r="P25" s="71"/>
-      <c r="Q25" s="71"/>
-      <c r="R25" s="71"/>
-      <c r="S25" s="71"/>
-      <c r="T25" s="71"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="75"/>
+      <c r="J25" s="75"/>
+      <c r="K25" s="75"/>
+      <c r="L25" s="75"/>
+      <c r="M25" s="75"/>
+      <c r="N25" s="76"/>
+      <c r="P25" s="81"/>
+      <c r="Q25" s="81"/>
+      <c r="R25" s="81"/>
+      <c r="S25" s="81"/>
+      <c r="T25" s="81"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B26" s="77"/>
-      <c r="C26" s="78"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="78"/>
-      <c r="I26" s="78"/>
-      <c r="J26" s="78"/>
-      <c r="K26" s="78"/>
-      <c r="L26" s="78"/>
-      <c r="M26" s="78"/>
-      <c r="N26" s="79"/>
-      <c r="P26" s="71"/>
-      <c r="Q26" s="71"/>
-      <c r="R26" s="71"/>
-      <c r="S26" s="71"/>
-      <c r="T26" s="71"/>
+      <c r="B26" s="74"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="75"/>
+      <c r="J26" s="75"/>
+      <c r="K26" s="75"/>
+      <c r="L26" s="75"/>
+      <c r="M26" s="75"/>
+      <c r="N26" s="76"/>
+      <c r="P26" s="81"/>
+      <c r="Q26" s="81"/>
+      <c r="R26" s="81"/>
+      <c r="S26" s="81"/>
+      <c r="T26" s="81"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B27" s="77"/>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="78"/>
-      <c r="I27" s="78"/>
-      <c r="J27" s="78"/>
-      <c r="K27" s="78"/>
-      <c r="L27" s="78"/>
-      <c r="M27" s="78"/>
-      <c r="N27" s="79"/>
-      <c r="P27" s="71"/>
-      <c r="Q27" s="71"/>
-      <c r="R27" s="71"/>
-      <c r="S27" s="71"/>
-      <c r="T27" s="71"/>
+      <c r="B27" s="74"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
+      <c r="J27" s="75"/>
+      <c r="K27" s="75"/>
+      <c r="L27" s="75"/>
+      <c r="M27" s="75"/>
+      <c r="N27" s="76"/>
+      <c r="P27" s="81"/>
+      <c r="Q27" s="81"/>
+      <c r="R27" s="81"/>
+      <c r="S27" s="81"/>
+      <c r="T27" s="81"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B28" s="77"/>
-      <c r="C28" s="78"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="78"/>
-      <c r="H28" s="78"/>
-      <c r="I28" s="78"/>
-      <c r="J28" s="78"/>
-      <c r="K28" s="78"/>
-      <c r="L28" s="78"/>
-      <c r="M28" s="78"/>
-      <c r="N28" s="79"/>
-      <c r="P28" s="71"/>
-      <c r="Q28" s="71"/>
-      <c r="R28" s="71"/>
-      <c r="S28" s="71"/>
-      <c r="T28" s="71"/>
+      <c r="B28" s="74"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="75"/>
+      <c r="J28" s="75"/>
+      <c r="K28" s="75"/>
+      <c r="L28" s="75"/>
+      <c r="M28" s="75"/>
+      <c r="N28" s="76"/>
+      <c r="P28" s="81"/>
+      <c r="Q28" s="81"/>
+      <c r="R28" s="81"/>
+      <c r="S28" s="81"/>
+      <c r="T28" s="81"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B29" s="77"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="78"/>
-      <c r="I29" s="78"/>
-      <c r="J29" s="78"/>
-      <c r="K29" s="78"/>
-      <c r="L29" s="78"/>
-      <c r="M29" s="78"/>
-      <c r="N29" s="79"/>
-      <c r="P29" s="71"/>
-      <c r="Q29" s="71"/>
-      <c r="R29" s="71"/>
-      <c r="S29" s="71"/>
-      <c r="T29" s="71"/>
+      <c r="B29" s="74"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="75"/>
+      <c r="J29" s="75"/>
+      <c r="K29" s="75"/>
+      <c r="L29" s="75"/>
+      <c r="M29" s="75"/>
+      <c r="N29" s="76"/>
+      <c r="P29" s="81"/>
+      <c r="Q29" s="81"/>
+      <c r="R29" s="81"/>
+      <c r="S29" s="81"/>
+      <c r="T29" s="81"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B30" s="77"/>
-      <c r="C30" s="78"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="78"/>
-      <c r="H30" s="78"/>
-      <c r="I30" s="78"/>
-      <c r="J30" s="78"/>
-      <c r="K30" s="78"/>
-      <c r="L30" s="78"/>
-      <c r="M30" s="78"/>
-      <c r="N30" s="79"/>
-      <c r="P30" s="71"/>
-      <c r="Q30" s="71"/>
-      <c r="R30" s="71"/>
-      <c r="S30" s="71"/>
-      <c r="T30" s="71"/>
+      <c r="B30" s="74"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="75"/>
+      <c r="I30" s="75"/>
+      <c r="J30" s="75"/>
+      <c r="K30" s="75"/>
+      <c r="L30" s="75"/>
+      <c r="M30" s="75"/>
+      <c r="N30" s="76"/>
+      <c r="P30" s="81"/>
+      <c r="Q30" s="81"/>
+      <c r="R30" s="81"/>
+      <c r="S30" s="81"/>
+      <c r="T30" s="81"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B31" s="77"/>
-      <c r="C31" s="78"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="78"/>
-      <c r="I31" s="78"/>
-      <c r="J31" s="78"/>
-      <c r="K31" s="78"/>
-      <c r="L31" s="78"/>
-      <c r="M31" s="78"/>
-      <c r="N31" s="79"/>
-      <c r="P31" s="71"/>
-      <c r="Q31" s="71"/>
-      <c r="R31" s="71"/>
-      <c r="S31" s="71"/>
-      <c r="T31" s="71"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="75"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="75"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="75"/>
+      <c r="H31" s="75"/>
+      <c r="I31" s="75"/>
+      <c r="J31" s="75"/>
+      <c r="K31" s="75"/>
+      <c r="L31" s="75"/>
+      <c r="M31" s="75"/>
+      <c r="N31" s="76"/>
+      <c r="P31" s="81"/>
+      <c r="Q31" s="81"/>
+      <c r="R31" s="81"/>
+      <c r="S31" s="81"/>
+      <c r="T31" s="81"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B32" s="77"/>
-      <c r="C32" s="78"/>
-      <c r="D32" s="78"/>
-      <c r="E32" s="78"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
-      <c r="H32" s="78"/>
-      <c r="I32" s="78"/>
-      <c r="J32" s="78"/>
-      <c r="K32" s="78"/>
-      <c r="L32" s="78"/>
-      <c r="M32" s="78"/>
-      <c r="N32" s="79"/>
-      <c r="P32" s="71"/>
-      <c r="Q32" s="71"/>
-      <c r="R32" s="71"/>
-      <c r="S32" s="71"/>
-      <c r="T32" s="71"/>
+      <c r="B32" s="74"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="75"/>
+      <c r="H32" s="75"/>
+      <c r="I32" s="75"/>
+      <c r="J32" s="75"/>
+      <c r="K32" s="75"/>
+      <c r="L32" s="75"/>
+      <c r="M32" s="75"/>
+      <c r="N32" s="76"/>
+      <c r="P32" s="81"/>
+      <c r="Q32" s="81"/>
+      <c r="R32" s="81"/>
+      <c r="S32" s="81"/>
+      <c r="T32" s="81"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B33" s="77"/>
-      <c r="C33" s="78"/>
-      <c r="D33" s="78"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="78"/>
-      <c r="H33" s="78"/>
-      <c r="I33" s="78"/>
-      <c r="J33" s="78"/>
-      <c r="K33" s="78"/>
-      <c r="L33" s="78"/>
-      <c r="M33" s="78"/>
-      <c r="N33" s="79"/>
-      <c r="P33" s="71"/>
-      <c r="Q33" s="71"/>
-      <c r="R33" s="71"/>
-      <c r="S33" s="71"/>
-      <c r="T33" s="71"/>
+      <c r="B33" s="74"/>
+      <c r="C33" s="75"/>
+      <c r="D33" s="75"/>
+      <c r="E33" s="75"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="75"/>
+      <c r="I33" s="75"/>
+      <c r="J33" s="75"/>
+      <c r="K33" s="75"/>
+      <c r="L33" s="75"/>
+      <c r="M33" s="75"/>
+      <c r="N33" s="76"/>
+      <c r="P33" s="81"/>
+      <c r="Q33" s="81"/>
+      <c r="R33" s="81"/>
+      <c r="S33" s="81"/>
+      <c r="T33" s="81"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B34" s="77"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="78"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78"/>
-      <c r="J34" s="78"/>
-      <c r="K34" s="78"/>
-      <c r="L34" s="78"/>
-      <c r="M34" s="78"/>
-      <c r="N34" s="79"/>
-      <c r="P34" s="71"/>
-      <c r="Q34" s="71"/>
-      <c r="R34" s="71"/>
-      <c r="S34" s="71"/>
-      <c r="T34" s="71"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="75"/>
+      <c r="F34" s="75"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="75"/>
+      <c r="I34" s="75"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="75"/>
+      <c r="L34" s="75"/>
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="P34" s="81"/>
+      <c r="Q34" s="81"/>
+      <c r="R34" s="81"/>
+      <c r="S34" s="81"/>
+      <c r="T34" s="81"/>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B35" s="77"/>
-      <c r="C35" s="78"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="78"/>
-      <c r="H35" s="78"/>
-      <c r="I35" s="78"/>
-      <c r="J35" s="78"/>
-      <c r="K35" s="78"/>
-      <c r="L35" s="78"/>
-      <c r="M35" s="78"/>
-      <c r="N35" s="79"/>
-      <c r="P35" s="71"/>
-      <c r="Q35" s="71"/>
-      <c r="R35" s="71"/>
-      <c r="S35" s="71"/>
-      <c r="T35" s="71"/>
+      <c r="B35" s="74"/>
+      <c r="C35" s="75"/>
+      <c r="D35" s="75"/>
+      <c r="E35" s="75"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="75"/>
+      <c r="H35" s="75"/>
+      <c r="I35" s="75"/>
+      <c r="J35" s="75"/>
+      <c r="K35" s="75"/>
+      <c r="L35" s="75"/>
+      <c r="M35" s="75"/>
+      <c r="N35" s="76"/>
+      <c r="P35" s="81"/>
+      <c r="Q35" s="81"/>
+      <c r="R35" s="81"/>
+      <c r="S35" s="81"/>
+      <c r="T35" s="81"/>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B36" s="77"/>
-      <c r="C36" s="78"/>
-      <c r="D36" s="78"/>
-      <c r="E36" s="78"/>
-      <c r="F36" s="78"/>
-      <c r="G36" s="78"/>
-      <c r="H36" s="78"/>
-      <c r="I36" s="78"/>
-      <c r="J36" s="78"/>
-      <c r="K36" s="78"/>
-      <c r="L36" s="78"/>
-      <c r="M36" s="78"/>
-      <c r="N36" s="79"/>
-      <c r="P36" s="71"/>
-      <c r="Q36" s="71"/>
-      <c r="R36" s="71"/>
-      <c r="S36" s="71"/>
-      <c r="T36" s="71"/>
+      <c r="B36" s="74"/>
+      <c r="C36" s="75"/>
+      <c r="D36" s="75"/>
+      <c r="E36" s="75"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="75"/>
+      <c r="I36" s="75"/>
+      <c r="J36" s="75"/>
+      <c r="K36" s="75"/>
+      <c r="L36" s="75"/>
+      <c r="M36" s="75"/>
+      <c r="N36" s="76"/>
+      <c r="P36" s="81"/>
+      <c r="Q36" s="81"/>
+      <c r="R36" s="81"/>
+      <c r="S36" s="81"/>
+      <c r="T36" s="81"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B37" s="77"/>
-      <c r="C37" s="78"/>
-      <c r="D37" s="78"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="78"/>
-      <c r="I37" s="78"/>
-      <c r="J37" s="78"/>
-      <c r="K37" s="78"/>
-      <c r="L37" s="78"/>
-      <c r="M37" s="78"/>
-      <c r="N37" s="79"/>
-      <c r="P37" s="71"/>
-      <c r="Q37" s="71"/>
-      <c r="R37" s="71"/>
-      <c r="S37" s="71"/>
-      <c r="T37" s="71"/>
+      <c r="B37" s="74"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
+      <c r="H37" s="75"/>
+      <c r="I37" s="75"/>
+      <c r="J37" s="75"/>
+      <c r="K37" s="75"/>
+      <c r="L37" s="75"/>
+      <c r="M37" s="75"/>
+      <c r="N37" s="76"/>
+      <c r="P37" s="81"/>
+      <c r="Q37" s="81"/>
+      <c r="R37" s="81"/>
+      <c r="S37" s="81"/>
+      <c r="T37" s="81"/>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B38" s="77"/>
-      <c r="C38" s="78"/>
-      <c r="D38" s="78"/>
-      <c r="E38" s="78"/>
-      <c r="F38" s="78"/>
-      <c r="G38" s="78"/>
-      <c r="H38" s="78"/>
-      <c r="I38" s="78"/>
-      <c r="J38" s="78"/>
-      <c r="K38" s="78"/>
-      <c r="L38" s="78"/>
-      <c r="M38" s="78"/>
-      <c r="N38" s="79"/>
-      <c r="P38" s="71"/>
-      <c r="Q38" s="71"/>
-      <c r="R38" s="71"/>
-      <c r="S38" s="71"/>
-      <c r="T38" s="71"/>
+      <c r="B38" s="74"/>
+      <c r="C38" s="75"/>
+      <c r="D38" s="75"/>
+      <c r="E38" s="75"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="75"/>
+      <c r="H38" s="75"/>
+      <c r="I38" s="75"/>
+      <c r="J38" s="75"/>
+      <c r="K38" s="75"/>
+      <c r="L38" s="75"/>
+      <c r="M38" s="75"/>
+      <c r="N38" s="76"/>
+      <c r="P38" s="81"/>
+      <c r="Q38" s="81"/>
+      <c r="R38" s="81"/>
+      <c r="S38" s="81"/>
+      <c r="T38" s="81"/>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B39" s="77"/>
-      <c r="C39" s="78"/>
-      <c r="D39" s="78"/>
-      <c r="E39" s="78"/>
-      <c r="F39" s="78"/>
-      <c r="G39" s="78"/>
-      <c r="H39" s="78"/>
-      <c r="I39" s="78"/>
-      <c r="J39" s="78"/>
-      <c r="K39" s="78"/>
-      <c r="L39" s="78"/>
-      <c r="M39" s="78"/>
-      <c r="N39" s="79"/>
-      <c r="P39" s="71"/>
-      <c r="Q39" s="71"/>
-      <c r="R39" s="71"/>
-      <c r="S39" s="71"/>
-      <c r="T39" s="71"/>
+      <c r="B39" s="74"/>
+      <c r="C39" s="75"/>
+      <c r="D39" s="75"/>
+      <c r="E39" s="75"/>
+      <c r="F39" s="75"/>
+      <c r="G39" s="75"/>
+      <c r="H39" s="75"/>
+      <c r="I39" s="75"/>
+      <c r="J39" s="75"/>
+      <c r="K39" s="75"/>
+      <c r="L39" s="75"/>
+      <c r="M39" s="75"/>
+      <c r="N39" s="76"/>
+      <c r="P39" s="81"/>
+      <c r="Q39" s="81"/>
+      <c r="R39" s="81"/>
+      <c r="S39" s="81"/>
+      <c r="T39" s="81"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B40" s="77"/>
-      <c r="C40" s="78"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="78"/>
-      <c r="F40" s="78"/>
-      <c r="G40" s="78"/>
-      <c r="H40" s="78"/>
-      <c r="I40" s="78"/>
-      <c r="J40" s="78"/>
-      <c r="K40" s="78"/>
-      <c r="L40" s="78"/>
-      <c r="M40" s="78"/>
-      <c r="N40" s="79"/>
-      <c r="P40" s="71"/>
-      <c r="Q40" s="71"/>
-      <c r="R40" s="71"/>
-      <c r="S40" s="71"/>
-      <c r="T40" s="71"/>
+      <c r="B40" s="74"/>
+      <c r="C40" s="75"/>
+      <c r="D40" s="75"/>
+      <c r="E40" s="75"/>
+      <c r="F40" s="75"/>
+      <c r="G40" s="75"/>
+      <c r="H40" s="75"/>
+      <c r="I40" s="75"/>
+      <c r="J40" s="75"/>
+      <c r="K40" s="75"/>
+      <c r="L40" s="75"/>
+      <c r="M40" s="75"/>
+      <c r="N40" s="76"/>
+      <c r="P40" s="81"/>
+      <c r="Q40" s="81"/>
+      <c r="R40" s="81"/>
+      <c r="S40" s="81"/>
+      <c r="T40" s="81"/>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B41" s="77"/>
-      <c r="C41" s="78"/>
-      <c r="D41" s="78"/>
-      <c r="E41" s="78"/>
-      <c r="F41" s="78"/>
-      <c r="G41" s="78"/>
-      <c r="H41" s="78"/>
-      <c r="I41" s="78"/>
-      <c r="J41" s="78"/>
-      <c r="K41" s="78"/>
-      <c r="L41" s="78"/>
-      <c r="M41" s="78"/>
-      <c r="N41" s="79"/>
-      <c r="P41" s="71"/>
-      <c r="Q41" s="71"/>
-      <c r="R41" s="71"/>
-      <c r="S41" s="71"/>
-      <c r="T41" s="71"/>
+      <c r="B41" s="74"/>
+      <c r="C41" s="75"/>
+      <c r="D41" s="75"/>
+      <c r="E41" s="75"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="75"/>
+      <c r="H41" s="75"/>
+      <c r="I41" s="75"/>
+      <c r="J41" s="75"/>
+      <c r="K41" s="75"/>
+      <c r="L41" s="75"/>
+      <c r="M41" s="75"/>
+      <c r="N41" s="76"/>
+      <c r="P41" s="81"/>
+      <c r="Q41" s="81"/>
+      <c r="R41" s="81"/>
+      <c r="S41" s="81"/>
+      <c r="T41" s="81"/>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B42" s="77"/>
-      <c r="C42" s="78"/>
-      <c r="D42" s="78"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="78"/>
-      <c r="G42" s="78"/>
-      <c r="H42" s="78"/>
-      <c r="I42" s="78"/>
-      <c r="J42" s="78"/>
-      <c r="K42" s="78"/>
-      <c r="L42" s="78"/>
-      <c r="M42" s="78"/>
-      <c r="N42" s="79"/>
-      <c r="P42" s="71"/>
-      <c r="Q42" s="71"/>
-      <c r="R42" s="71"/>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
+      <c r="B42" s="74"/>
+      <c r="C42" s="75"/>
+      <c r="D42" s="75"/>
+      <c r="E42" s="75"/>
+      <c r="F42" s="75"/>
+      <c r="G42" s="75"/>
+      <c r="H42" s="75"/>
+      <c r="I42" s="75"/>
+      <c r="J42" s="75"/>
+      <c r="K42" s="75"/>
+      <c r="L42" s="75"/>
+      <c r="M42" s="75"/>
+      <c r="N42" s="76"/>
+      <c r="P42" s="81"/>
+      <c r="Q42" s="81"/>
+      <c r="R42" s="81"/>
+      <c r="S42" s="81"/>
+      <c r="T42" s="81"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B43" s="77"/>
-      <c r="C43" s="78"/>
-      <c r="D43" s="78"/>
-      <c r="E43" s="78"/>
-      <c r="F43" s="78"/>
-      <c r="G43" s="78"/>
-      <c r="H43" s="78"/>
-      <c r="I43" s="78"/>
-      <c r="J43" s="78"/>
-      <c r="K43" s="78"/>
-      <c r="L43" s="78"/>
-      <c r="M43" s="78"/>
-      <c r="N43" s="79"/>
-      <c r="P43" s="71"/>
-      <c r="Q43" s="71"/>
-      <c r="R43" s="71"/>
-      <c r="S43" s="71"/>
-      <c r="T43" s="71"/>
+      <c r="B43" s="74"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="75"/>
+      <c r="F43" s="75"/>
+      <c r="G43" s="75"/>
+      <c r="H43" s="75"/>
+      <c r="I43" s="75"/>
+      <c r="J43" s="75"/>
+      <c r="K43" s="75"/>
+      <c r="L43" s="75"/>
+      <c r="M43" s="75"/>
+      <c r="N43" s="76"/>
+      <c r="P43" s="81"/>
+      <c r="Q43" s="81"/>
+      <c r="R43" s="81"/>
+      <c r="S43" s="81"/>
+      <c r="T43" s="81"/>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B44" s="80"/>
-      <c r="C44" s="81"/>
-      <c r="D44" s="81"/>
-      <c r="E44" s="81"/>
-      <c r="F44" s="81"/>
-      <c r="G44" s="81"/>
-      <c r="H44" s="81"/>
-      <c r="I44" s="81"/>
-      <c r="J44" s="81"/>
-      <c r="K44" s="81"/>
-      <c r="L44" s="81"/>
-      <c r="M44" s="81"/>
-      <c r="N44" s="82"/>
-      <c r="P44" s="71"/>
-      <c r="Q44" s="71"/>
-      <c r="R44" s="71"/>
-      <c r="S44" s="71"/>
-      <c r="T44" s="71"/>
+      <c r="B44" s="77"/>
+      <c r="C44" s="78"/>
+      <c r="D44" s="78"/>
+      <c r="E44" s="78"/>
+      <c r="F44" s="78"/>
+      <c r="G44" s="78"/>
+      <c r="H44" s="78"/>
+      <c r="I44" s="78"/>
+      <c r="J44" s="78"/>
+      <c r="K44" s="78"/>
+      <c r="L44" s="78"/>
+      <c r="M44" s="78"/>
+      <c r="N44" s="79"/>
+      <c r="P44" s="81"/>
+      <c r="Q44" s="81"/>
+      <c r="R44" s="81"/>
+      <c r="S44" s="81"/>
+      <c r="T44" s="81"/>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B45" s="72" t="s">
+      <c r="B45" s="70" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="72"/>
-      <c r="D45" s="72"/>
-      <c r="E45" s="72"/>
-      <c r="F45" s="72"/>
-      <c r="G45" s="72"/>
-      <c r="H45" s="72"/>
-      <c r="I45" s="72"/>
-      <c r="J45" s="72"/>
-      <c r="K45" s="72"/>
-      <c r="L45" s="72"/>
-      <c r="M45" s="72"/>
-      <c r="N45" s="72"/>
+      <c r="C45" s="70"/>
+      <c r="D45" s="70"/>
+      <c r="E45" s="70"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="70"/>
+      <c r="H45" s="70"/>
+      <c r="I45" s="70"/>
+      <c r="J45" s="70"/>
+      <c r="K45" s="70"/>
+      <c r="L45" s="70"/>
+      <c r="M45" s="70"/>
+      <c r="N45" s="70"/>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B46" s="74"/>
-      <c r="C46" s="75"/>
-      <c r="D46" s="75"/>
-      <c r="E46" s="75"/>
-      <c r="F46" s="75"/>
-      <c r="G46" s="75"/>
-      <c r="H46" s="75"/>
-      <c r="I46" s="75"/>
-      <c r="J46" s="75"/>
-      <c r="K46" s="75"/>
-      <c r="L46" s="75"/>
-      <c r="M46" s="75"/>
-      <c r="N46" s="76"/>
+      <c r="B46" s="71"/>
+      <c r="C46" s="72"/>
+      <c r="D46" s="72"/>
+      <c r="E46" s="72"/>
+      <c r="F46" s="72"/>
+      <c r="G46" s="72"/>
+      <c r="H46" s="72"/>
+      <c r="I46" s="72"/>
+      <c r="J46" s="72"/>
+      <c r="K46" s="72"/>
+      <c r="L46" s="72"/>
+      <c r="M46" s="72"/>
+      <c r="N46" s="73"/>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B47" s="77"/>
-      <c r="C47" s="78"/>
-      <c r="D47" s="78"/>
-      <c r="E47" s="78"/>
-      <c r="F47" s="78"/>
-      <c r="G47" s="78"/>
-      <c r="H47" s="78"/>
-      <c r="I47" s="78"/>
-      <c r="J47" s="78"/>
-      <c r="K47" s="78"/>
-      <c r="L47" s="78"/>
-      <c r="M47" s="78"/>
-      <c r="N47" s="79"/>
+      <c r="B47" s="74"/>
+      <c r="C47" s="75"/>
+      <c r="D47" s="75"/>
+      <c r="E47" s="75"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="75"/>
+      <c r="H47" s="75"/>
+      <c r="I47" s="75"/>
+      <c r="J47" s="75"/>
+      <c r="K47" s="75"/>
+      <c r="L47" s="75"/>
+      <c r="M47" s="75"/>
+      <c r="N47" s="76"/>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B48" s="77"/>
-      <c r="C48" s="78"/>
-      <c r="D48" s="78"/>
-      <c r="E48" s="78"/>
-      <c r="F48" s="78"/>
-      <c r="G48" s="78"/>
-      <c r="H48" s="78"/>
-      <c r="I48" s="78"/>
-      <c r="J48" s="78"/>
-      <c r="K48" s="78"/>
-      <c r="L48" s="78"/>
-      <c r="M48" s="78"/>
-      <c r="N48" s="79"/>
+      <c r="B48" s="74"/>
+      <c r="C48" s="75"/>
+      <c r="D48" s="75"/>
+      <c r="E48" s="75"/>
+      <c r="F48" s="75"/>
+      <c r="G48" s="75"/>
+      <c r="H48" s="75"/>
+      <c r="I48" s="75"/>
+      <c r="J48" s="75"/>
+      <c r="K48" s="75"/>
+      <c r="L48" s="75"/>
+      <c r="M48" s="75"/>
+      <c r="N48" s="76"/>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B49" s="77"/>
-      <c r="C49" s="78"/>
-      <c r="D49" s="78"/>
-      <c r="E49" s="78"/>
-      <c r="F49" s="78"/>
-      <c r="G49" s="78"/>
-      <c r="H49" s="78"/>
-      <c r="I49" s="78"/>
-      <c r="J49" s="78"/>
-      <c r="K49" s="78"/>
-      <c r="L49" s="78"/>
-      <c r="M49" s="78"/>
-      <c r="N49" s="79"/>
+      <c r="B49" s="74"/>
+      <c r="C49" s="75"/>
+      <c r="D49" s="75"/>
+      <c r="E49" s="75"/>
+      <c r="F49" s="75"/>
+      <c r="G49" s="75"/>
+      <c r="H49" s="75"/>
+      <c r="I49" s="75"/>
+      <c r="J49" s="75"/>
+      <c r="K49" s="75"/>
+      <c r="L49" s="75"/>
+      <c r="M49" s="75"/>
+      <c r="N49" s="76"/>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B50" s="77"/>
-      <c r="C50" s="78"/>
-      <c r="D50" s="78"/>
-      <c r="E50" s="78"/>
-      <c r="F50" s="78"/>
-      <c r="G50" s="78"/>
-      <c r="H50" s="78"/>
-      <c r="I50" s="78"/>
-      <c r="J50" s="78"/>
-      <c r="K50" s="78"/>
-      <c r="L50" s="78"/>
-      <c r="M50" s="78"/>
-      <c r="N50" s="79"/>
+      <c r="B50" s="74"/>
+      <c r="C50" s="75"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="75"/>
+      <c r="F50" s="75"/>
+      <c r="G50" s="75"/>
+      <c r="H50" s="75"/>
+      <c r="I50" s="75"/>
+      <c r="J50" s="75"/>
+      <c r="K50" s="75"/>
+      <c r="L50" s="75"/>
+      <c r="M50" s="75"/>
+      <c r="N50" s="76"/>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B51" s="77"/>
-      <c r="C51" s="78"/>
-      <c r="D51" s="78"/>
-      <c r="E51" s="78"/>
-      <c r="F51" s="78"/>
-      <c r="G51" s="78"/>
-      <c r="H51" s="78"/>
-      <c r="I51" s="78"/>
-      <c r="J51" s="78"/>
-      <c r="K51" s="78"/>
-      <c r="L51" s="78"/>
-      <c r="M51" s="78"/>
-      <c r="N51" s="79"/>
+      <c r="B51" s="74"/>
+      <c r="C51" s="75"/>
+      <c r="D51" s="75"/>
+      <c r="E51" s="75"/>
+      <c r="F51" s="75"/>
+      <c r="G51" s="75"/>
+      <c r="H51" s="75"/>
+      <c r="I51" s="75"/>
+      <c r="J51" s="75"/>
+      <c r="K51" s="75"/>
+      <c r="L51" s="75"/>
+      <c r="M51" s="75"/>
+      <c r="N51" s="76"/>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B52" s="77"/>
-      <c r="C52" s="78"/>
-      <c r="D52" s="78"/>
-      <c r="E52" s="78"/>
-      <c r="F52" s="78"/>
-      <c r="G52" s="78"/>
-      <c r="H52" s="78"/>
-      <c r="I52" s="78"/>
-      <c r="J52" s="78"/>
-      <c r="K52" s="78"/>
-      <c r="L52" s="78"/>
-      <c r="M52" s="78"/>
-      <c r="N52" s="79"/>
+      <c r="B52" s="74"/>
+      <c r="C52" s="75"/>
+      <c r="D52" s="75"/>
+      <c r="E52" s="75"/>
+      <c r="F52" s="75"/>
+      <c r="G52" s="75"/>
+      <c r="H52" s="75"/>
+      <c r="I52" s="75"/>
+      <c r="J52" s="75"/>
+      <c r="K52" s="75"/>
+      <c r="L52" s="75"/>
+      <c r="M52" s="75"/>
+      <c r="N52" s="76"/>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B53" s="77"/>
-      <c r="C53" s="78"/>
-      <c r="D53" s="78"/>
-      <c r="E53" s="78"/>
-      <c r="F53" s="78"/>
-      <c r="G53" s="78"/>
-      <c r="H53" s="78"/>
-      <c r="I53" s="78"/>
-      <c r="J53" s="78"/>
-      <c r="K53" s="78"/>
-      <c r="L53" s="78"/>
-      <c r="M53" s="78"/>
-      <c r="N53" s="79"/>
+      <c r="B53" s="74"/>
+      <c r="C53" s="75"/>
+      <c r="D53" s="75"/>
+      <c r="E53" s="75"/>
+      <c r="F53" s="75"/>
+      <c r="G53" s="75"/>
+      <c r="H53" s="75"/>
+      <c r="I53" s="75"/>
+      <c r="J53" s="75"/>
+      <c r="K53" s="75"/>
+      <c r="L53" s="75"/>
+      <c r="M53" s="75"/>
+      <c r="N53" s="76"/>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B54" s="77"/>
-      <c r="C54" s="78"/>
-      <c r="D54" s="78"/>
-      <c r="E54" s="78"/>
-      <c r="F54" s="78"/>
-      <c r="G54" s="78"/>
-      <c r="H54" s="78"/>
-      <c r="I54" s="78"/>
-      <c r="J54" s="78"/>
-      <c r="K54" s="78"/>
-      <c r="L54" s="78"/>
-      <c r="M54" s="78"/>
-      <c r="N54" s="79"/>
+      <c r="B54" s="74"/>
+      <c r="C54" s="75"/>
+      <c r="D54" s="75"/>
+      <c r="E54" s="75"/>
+      <c r="F54" s="75"/>
+      <c r="G54" s="75"/>
+      <c r="H54" s="75"/>
+      <c r="I54" s="75"/>
+      <c r="J54" s="75"/>
+      <c r="K54" s="75"/>
+      <c r="L54" s="75"/>
+      <c r="M54" s="75"/>
+      <c r="N54" s="76"/>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B55" s="77"/>
-      <c r="C55" s="78"/>
-      <c r="D55" s="78"/>
-      <c r="E55" s="78"/>
-      <c r="F55" s="78"/>
-      <c r="G55" s="78"/>
-      <c r="H55" s="78"/>
-      <c r="I55" s="78"/>
-      <c r="J55" s="78"/>
-      <c r="K55" s="78"/>
-      <c r="L55" s="78"/>
-      <c r="M55" s="78"/>
-      <c r="N55" s="79"/>
+      <c r="B55" s="74"/>
+      <c r="C55" s="75"/>
+      <c r="D55" s="75"/>
+      <c r="E55" s="75"/>
+      <c r="F55" s="75"/>
+      <c r="G55" s="75"/>
+      <c r="H55" s="75"/>
+      <c r="I55" s="75"/>
+      <c r="J55" s="75"/>
+      <c r="K55" s="75"/>
+      <c r="L55" s="75"/>
+      <c r="M55" s="75"/>
+      <c r="N55" s="76"/>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B56" s="77"/>
-      <c r="C56" s="78"/>
-      <c r="D56" s="78"/>
-      <c r="E56" s="78"/>
-      <c r="F56" s="78"/>
-      <c r="G56" s="78"/>
-      <c r="H56" s="78"/>
-      <c r="I56" s="78"/>
-      <c r="J56" s="78"/>
-      <c r="K56" s="78"/>
-      <c r="L56" s="78"/>
-      <c r="M56" s="78"/>
-      <c r="N56" s="79"/>
+      <c r="B56" s="74"/>
+      <c r="C56" s="75"/>
+      <c r="D56" s="75"/>
+      <c r="E56" s="75"/>
+      <c r="F56" s="75"/>
+      <c r="G56" s="75"/>
+      <c r="H56" s="75"/>
+      <c r="I56" s="75"/>
+      <c r="J56" s="75"/>
+      <c r="K56" s="75"/>
+      <c r="L56" s="75"/>
+      <c r="M56" s="75"/>
+      <c r="N56" s="76"/>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B57" s="77"/>
-      <c r="C57" s="78"/>
-      <c r="D57" s="78"/>
-      <c r="E57" s="78"/>
-      <c r="F57" s="78"/>
-      <c r="G57" s="78"/>
-      <c r="H57" s="78"/>
-      <c r="I57" s="78"/>
-      <c r="J57" s="78"/>
-      <c r="K57" s="78"/>
-      <c r="L57" s="78"/>
-      <c r="M57" s="78"/>
-      <c r="N57" s="79"/>
+      <c r="B57" s="74"/>
+      <c r="C57" s="75"/>
+      <c r="D57" s="75"/>
+      <c r="E57" s="75"/>
+      <c r="F57" s="75"/>
+      <c r="G57" s="75"/>
+      <c r="H57" s="75"/>
+      <c r="I57" s="75"/>
+      <c r="J57" s="75"/>
+      <c r="K57" s="75"/>
+      <c r="L57" s="75"/>
+      <c r="M57" s="75"/>
+      <c r="N57" s="76"/>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B58" s="77"/>
-      <c r="C58" s="78"/>
-      <c r="D58" s="78"/>
-      <c r="E58" s="78"/>
-      <c r="F58" s="78"/>
-      <c r="G58" s="78"/>
-      <c r="H58" s="78"/>
-      <c r="I58" s="78"/>
-      <c r="J58" s="78"/>
-      <c r="K58" s="78"/>
-      <c r="L58" s="78"/>
-      <c r="M58" s="78"/>
-      <c r="N58" s="79"/>
+      <c r="B58" s="74"/>
+      <c r="C58" s="75"/>
+      <c r="D58" s="75"/>
+      <c r="E58" s="75"/>
+      <c r="F58" s="75"/>
+      <c r="G58" s="75"/>
+      <c r="H58" s="75"/>
+      <c r="I58" s="75"/>
+      <c r="J58" s="75"/>
+      <c r="K58" s="75"/>
+      <c r="L58" s="75"/>
+      <c r="M58" s="75"/>
+      <c r="N58" s="76"/>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B59" s="77"/>
-      <c r="C59" s="78"/>
-      <c r="D59" s="78"/>
-      <c r="E59" s="78"/>
-      <c r="F59" s="78"/>
-      <c r="G59" s="78"/>
-      <c r="H59" s="78"/>
-      <c r="I59" s="78"/>
-      <c r="J59" s="78"/>
-      <c r="K59" s="78"/>
-      <c r="L59" s="78"/>
-      <c r="M59" s="78"/>
-      <c r="N59" s="79"/>
+      <c r="B59" s="74"/>
+      <c r="C59" s="75"/>
+      <c r="D59" s="75"/>
+      <c r="E59" s="75"/>
+      <c r="F59" s="75"/>
+      <c r="G59" s="75"/>
+      <c r="H59" s="75"/>
+      <c r="I59" s="75"/>
+      <c r="J59" s="75"/>
+      <c r="K59" s="75"/>
+      <c r="L59" s="75"/>
+      <c r="M59" s="75"/>
+      <c r="N59" s="76"/>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B60" s="77"/>
-      <c r="C60" s="78"/>
-      <c r="D60" s="78"/>
-      <c r="E60" s="78"/>
-      <c r="F60" s="78"/>
-      <c r="G60" s="78"/>
-      <c r="H60" s="78"/>
-      <c r="I60" s="78"/>
-      <c r="J60" s="78"/>
-      <c r="K60" s="78"/>
-      <c r="L60" s="78"/>
-      <c r="M60" s="78"/>
-      <c r="N60" s="79"/>
+      <c r="B60" s="74"/>
+      <c r="C60" s="75"/>
+      <c r="D60" s="75"/>
+      <c r="E60" s="75"/>
+      <c r="F60" s="75"/>
+      <c r="G60" s="75"/>
+      <c r="H60" s="75"/>
+      <c r="I60" s="75"/>
+      <c r="J60" s="75"/>
+      <c r="K60" s="75"/>
+      <c r="L60" s="75"/>
+      <c r="M60" s="75"/>
+      <c r="N60" s="76"/>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B61" s="77"/>
-      <c r="C61" s="78"/>
-      <c r="D61" s="78"/>
-      <c r="E61" s="78"/>
-      <c r="F61" s="78"/>
-      <c r="G61" s="78"/>
-      <c r="H61" s="78"/>
-      <c r="I61" s="78"/>
-      <c r="J61" s="78"/>
-      <c r="K61" s="78"/>
-      <c r="L61" s="78"/>
-      <c r="M61" s="78"/>
-      <c r="N61" s="79"/>
+      <c r="B61" s="74"/>
+      <c r="C61" s="75"/>
+      <c r="D61" s="75"/>
+      <c r="E61" s="75"/>
+      <c r="F61" s="75"/>
+      <c r="G61" s="75"/>
+      <c r="H61" s="75"/>
+      <c r="I61" s="75"/>
+      <c r="J61" s="75"/>
+      <c r="K61" s="75"/>
+      <c r="L61" s="75"/>
+      <c r="M61" s="75"/>
+      <c r="N61" s="76"/>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B62" s="77"/>
-      <c r="C62" s="78"/>
-      <c r="D62" s="78"/>
-      <c r="E62" s="78"/>
-      <c r="F62" s="78"/>
-      <c r="G62" s="78"/>
-      <c r="H62" s="78"/>
-      <c r="I62" s="78"/>
-      <c r="J62" s="78"/>
-      <c r="K62" s="78"/>
-      <c r="L62" s="78"/>
-      <c r="M62" s="78"/>
-      <c r="N62" s="79"/>
+      <c r="B62" s="74"/>
+      <c r="C62" s="75"/>
+      <c r="D62" s="75"/>
+      <c r="E62" s="75"/>
+      <c r="F62" s="75"/>
+      <c r="G62" s="75"/>
+      <c r="H62" s="75"/>
+      <c r="I62" s="75"/>
+      <c r="J62" s="75"/>
+      <c r="K62" s="75"/>
+      <c r="L62" s="75"/>
+      <c r="M62" s="75"/>
+      <c r="N62" s="76"/>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B63" s="77"/>
-      <c r="C63" s="78"/>
-      <c r="D63" s="78"/>
-      <c r="E63" s="78"/>
-      <c r="F63" s="78"/>
-      <c r="G63" s="78"/>
-      <c r="H63" s="78"/>
-      <c r="I63" s="78"/>
-      <c r="J63" s="78"/>
-      <c r="K63" s="78"/>
-      <c r="L63" s="78"/>
-      <c r="M63" s="78"/>
-      <c r="N63" s="79"/>
+      <c r="B63" s="74"/>
+      <c r="C63" s="75"/>
+      <c r="D63" s="75"/>
+      <c r="E63" s="75"/>
+      <c r="F63" s="75"/>
+      <c r="G63" s="75"/>
+      <c r="H63" s="75"/>
+      <c r="I63" s="75"/>
+      <c r="J63" s="75"/>
+      <c r="K63" s="75"/>
+      <c r="L63" s="75"/>
+      <c r="M63" s="75"/>
+      <c r="N63" s="76"/>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B64" s="77"/>
-      <c r="C64" s="78"/>
-      <c r="D64" s="78"/>
-      <c r="E64" s="78"/>
-      <c r="F64" s="78"/>
-      <c r="G64" s="78"/>
-      <c r="H64" s="78"/>
-      <c r="I64" s="78"/>
-      <c r="J64" s="78"/>
-      <c r="K64" s="78"/>
-      <c r="L64" s="78"/>
-      <c r="M64" s="78"/>
-      <c r="N64" s="79"/>
+      <c r="B64" s="74"/>
+      <c r="C64" s="75"/>
+      <c r="D64" s="75"/>
+      <c r="E64" s="75"/>
+      <c r="F64" s="75"/>
+      <c r="G64" s="75"/>
+      <c r="H64" s="75"/>
+      <c r="I64" s="75"/>
+      <c r="J64" s="75"/>
+      <c r="K64" s="75"/>
+      <c r="L64" s="75"/>
+      <c r="M64" s="75"/>
+      <c r="N64" s="76"/>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B65" s="77"/>
-      <c r="C65" s="78"/>
-      <c r="D65" s="78"/>
-      <c r="E65" s="78"/>
-      <c r="F65" s="78"/>
-      <c r="G65" s="78"/>
-      <c r="H65" s="78"/>
-      <c r="I65" s="78"/>
-      <c r="J65" s="78"/>
-      <c r="K65" s="78"/>
-      <c r="L65" s="78"/>
-      <c r="M65" s="78"/>
-      <c r="N65" s="79"/>
+      <c r="B65" s="74"/>
+      <c r="C65" s="75"/>
+      <c r="D65" s="75"/>
+      <c r="E65" s="75"/>
+      <c r="F65" s="75"/>
+      <c r="G65" s="75"/>
+      <c r="H65" s="75"/>
+      <c r="I65" s="75"/>
+      <c r="J65" s="75"/>
+      <c r="K65" s="75"/>
+      <c r="L65" s="75"/>
+      <c r="M65" s="75"/>
+      <c r="N65" s="76"/>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B66" s="77"/>
-      <c r="C66" s="78"/>
-      <c r="D66" s="78"/>
-      <c r="E66" s="78"/>
-      <c r="F66" s="78"/>
-      <c r="G66" s="78"/>
-      <c r="H66" s="78"/>
-      <c r="I66" s="78"/>
-      <c r="J66" s="78"/>
-      <c r="K66" s="78"/>
-      <c r="L66" s="78"/>
-      <c r="M66" s="78"/>
-      <c r="N66" s="79"/>
+      <c r="B66" s="74"/>
+      <c r="C66" s="75"/>
+      <c r="D66" s="75"/>
+      <c r="E66" s="75"/>
+      <c r="F66" s="75"/>
+      <c r="G66" s="75"/>
+      <c r="H66" s="75"/>
+      <c r="I66" s="75"/>
+      <c r="J66" s="75"/>
+      <c r="K66" s="75"/>
+      <c r="L66" s="75"/>
+      <c r="M66" s="75"/>
+      <c r="N66" s="76"/>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B67" s="77"/>
-      <c r="C67" s="78"/>
-      <c r="D67" s="78"/>
-      <c r="E67" s="78"/>
-      <c r="F67" s="78"/>
-      <c r="G67" s="78"/>
-      <c r="H67" s="78"/>
-      <c r="I67" s="78"/>
-      <c r="J67" s="78"/>
-      <c r="K67" s="78"/>
-      <c r="L67" s="78"/>
-      <c r="M67" s="78"/>
-      <c r="N67" s="79"/>
+      <c r="B67" s="74"/>
+      <c r="C67" s="75"/>
+      <c r="D67" s="75"/>
+      <c r="E67" s="75"/>
+      <c r="F67" s="75"/>
+      <c r="G67" s="75"/>
+      <c r="H67" s="75"/>
+      <c r="I67" s="75"/>
+      <c r="J67" s="75"/>
+      <c r="K67" s="75"/>
+      <c r="L67" s="75"/>
+      <c r="M67" s="75"/>
+      <c r="N67" s="76"/>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B68" s="80"/>
-      <c r="C68" s="81"/>
-      <c r="D68" s="81"/>
-      <c r="E68" s="81"/>
-      <c r="F68" s="81"/>
-      <c r="G68" s="81"/>
-      <c r="H68" s="81"/>
-      <c r="I68" s="81"/>
-      <c r="J68" s="81"/>
-      <c r="K68" s="81"/>
-      <c r="L68" s="81"/>
-      <c r="M68" s="81"/>
-      <c r="N68" s="82"/>
+      <c r="B68" s="77"/>
+      <c r="C68" s="78"/>
+      <c r="D68" s="78"/>
+      <c r="E68" s="78"/>
+      <c r="F68" s="78"/>
+      <c r="G68" s="78"/>
+      <c r="H68" s="78"/>
+      <c r="I68" s="78"/>
+      <c r="J68" s="78"/>
+      <c r="K68" s="78"/>
+      <c r="L68" s="78"/>
+      <c r="M68" s="78"/>
+      <c r="N68" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3520,20 +3525,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="F1" s="55" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="F1" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -3548,12 +3553,12 @@
       <c r="D2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
@@ -3568,12 +3573,12 @@
       <c r="D3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
@@ -3582,16 +3587,16 @@
       <c r="B4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="84"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
+      <c r="D4" s="89"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
     </row>
     <row r="5" spans="1:11" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -3600,16 +3605,16 @@
       <c r="B5" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="84" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="83"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
+      <c r="D5" s="84"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="94"/>
     </row>
     <row r="6" spans="1:11" s="29" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
@@ -3618,16 +3623,16 @@
       <c r="B6" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="94" t="s">
+      <c r="C6" s="91" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="95"/>
-      <c r="F6" s="91"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="91"/>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
+      <c r="D6" s="92"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="94"/>
+      <c r="K6" s="94"/>
     </row>
     <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
@@ -3636,16 +3641,16 @@
       <c r="B7" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="84" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="83"/>
-      <c r="F7" s="91"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="91"/>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91"/>
+      <c r="D7" s="84"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="94"/>
     </row>
     <row r="8" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
@@ -3654,16 +3659,16 @@
       <c r="B8" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="C8" s="93" t="s">
+      <c r="C8" s="90" t="s">
         <v>126</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="91"/>
-      <c r="I8" s="91"/>
-      <c r="J8" s="91"/>
-      <c r="K8" s="91"/>
+      <c r="D8" s="90"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="94"/>
     </row>
     <row r="9" spans="1:11" s="29" customFormat="1" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
@@ -3672,10 +3677,10 @@
       <c r="B9" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="94" t="s">
+      <c r="C9" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="95"/>
+      <c r="D9" s="92"/>
       <c r="F9" s="35"/>
       <c r="G9" s="35"/>
       <c r="H9" s="35"/>
@@ -3730,10 +3735,10 @@
       <c r="B12" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="84" t="s">
+      <c r="C12" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="84"/>
+      <c r="D12" s="89"/>
       <c r="F12" s="35"/>
       <c r="G12" s="35"/>
       <c r="H12" s="35"/>
@@ -3748,10 +3753,10 @@
       <c r="B13" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="89" t="s">
+      <c r="C13" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="89"/>
+      <c r="D13" s="95"/>
       <c r="F13" s="35"/>
       <c r="G13" s="35"/>
       <c r="H13" s="35"/>
@@ -3806,10 +3811,10 @@
       <c r="B16" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="84" t="s">
+      <c r="C16" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="84"/>
+      <c r="D16" s="89"/>
       <c r="F16" s="35"/>
       <c r="G16" s="35"/>
       <c r="H16" s="35"/>
@@ -3824,10 +3829,10 @@
       <c r="B17" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="C17" s="83" t="s">
+      <c r="C17" s="84" t="s">
         <v>129</v>
       </c>
-      <c r="D17" s="83"/>
+      <c r="D17" s="84"/>
       <c r="F17" s="35"/>
       <c r="G17" s="35"/>
       <c r="H17" s="35"/>
@@ -3882,10 +3887,10 @@
       <c r="B20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="90" t="s">
+      <c r="C20" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="90"/>
+      <c r="D20" s="93"/>
       <c r="F20" s="35"/>
       <c r="G20" s="35"/>
       <c r="H20" s="35"/>
@@ -3894,10 +3899,10 @@
       <c r="K20" s="35"/>
     </row>
     <row r="21" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="92" t="s">
+      <c r="A21" s="83" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="83" t="s">
+      <c r="B21" s="84" t="s">
         <v>133</v>
       </c>
       <c r="C21" s="85" t="s">
@@ -3912,8 +3917,8 @@
       <c r="K21" s="35"/>
     </row>
     <row r="22" spans="1:11" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="92"/>
-      <c r="B22" s="83"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="84"/>
       <c r="C22" s="87"/>
       <c r="D22" s="88"/>
       <c r="F22" s="21"/>
@@ -3924,10 +3929,10 @@
       <c r="K22" s="21"/>
     </row>
     <row r="23" spans="1:11" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="92" t="s">
+      <c r="A23" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="83" t="s">
+      <c r="B23" s="84" t="s">
         <v>76</v>
       </c>
       <c r="C23" s="85" t="s">
@@ -3936,8 +3941,8 @@
       <c r="D23" s="86"/>
     </row>
     <row r="24" spans="1:11" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="92"/>
-      <c r="B24" s="83"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="84"/>
       <c r="C24" s="87"/>
       <c r="D24" s="88"/>
     </row>
@@ -3948,10 +3953,10 @@
       <c r="B25" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="C25" s="83" t="s">
+      <c r="C25" s="84" t="s">
         <v>131</v>
       </c>
-      <c r="D25" s="83"/>
+      <c r="D25" s="84"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
@@ -3988,10 +3993,10 @@
       <c r="B28" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="84" t="s">
+      <c r="C28" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="84"/>
+      <c r="D28" s="89"/>
     </row>
     <row r="29" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
@@ -4000,10 +4005,10 @@
       <c r="B29" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="83" t="s">
+      <c r="C29" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="83"/>
+      <c r="D29" s="84"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="34" t="s">
@@ -4040,10 +4045,10 @@
       <c r="B32" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="84" t="s">
+      <c r="C32" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="84"/>
+      <c r="D32" s="89"/>
     </row>
     <row r="33" spans="1:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="31" t="s">
@@ -4052,10 +4057,10 @@
       <c r="B33" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="83" t="s">
+      <c r="C33" s="84" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="83"/>
+      <c r="D33" s="84"/>
     </row>
     <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="41" t="s">
@@ -4064,30 +4069,13 @@
       <c r="B34" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="83" t="s">
+      <c r="C34" s="84" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="83"/>
+      <c r="D34" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F2:K8"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="C33:D33"/>
@@ -4097,6 +4085,23 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C29:D29"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F2:K8"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4121,15 +4126,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">

</xml_diff>